<commit_message>
Final rankings with old model parameters
</commit_message>
<xml_diff>
--- a/output/CRAPPR - Top Matchups.xlsx
+++ b/output/CRAPPR - Top Matchups.xlsx
@@ -13,111 +13,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="51" uniqueCount="40">
-  <si>
-    <t>Arun / Zeeshan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="57" uniqueCount="43">
+  <si>
+    <t>Benael / Rowan</t>
+  </si>
+  <si>
+    <t>David_S / Matt</t>
+  </si>
+  <si>
+    <t>Ben / Jack</t>
+  </si>
+  <si>
+    <t>Cedric / Rowan</t>
+  </si>
+  <si>
+    <t>Benael / Matt</t>
+  </si>
+  <si>
+    <t>Arun / Benael</t>
+  </si>
+  <si>
+    <t>Ben / Vasisht</t>
+  </si>
+  <si>
+    <t>Arun / David_S</t>
+  </si>
+  <si>
+    <t>Cedric / Matt</t>
+  </si>
+  <si>
+    <t>Arun / Jack</t>
+  </si>
+  <si>
+    <t>Ben / Cedric</t>
+  </si>
+  <si>
+    <t>Arun / Cedric</t>
+  </si>
+  <si>
+    <t>David_S / Neil</t>
   </si>
   <si>
     <t>Ben / Benael</t>
   </si>
   <si>
+    <t>Arun / Neil</t>
+  </si>
+  <si>
+    <t>Andres / Rowan</t>
+  </si>
+  <si>
+    <t>Andres / Matt</t>
+  </si>
+  <si>
     <t>Jack / Neil</t>
   </si>
   <si>
-    <t>Arun / Matt</t>
-  </si>
-  <si>
-    <t>Andres / David_S</t>
-  </si>
-  <si>
     <t>Andres / Jack</t>
   </si>
   <si>
-    <t>Andres / Neil</t>
-  </si>
-  <si>
-    <t>Arun / Neil</t>
-  </si>
-  <si>
-    <t>Benael / Matt</t>
+    <t>Andres / Ben</t>
+  </si>
+  <si>
+    <t>David_S / Yumeng</t>
+  </si>
+  <si>
+    <t>Jack / Rowan</t>
   </si>
   <si>
     <t>David_S / Rowan</t>
   </si>
   <si>
-    <t>Ben / Victor</t>
-  </si>
-  <si>
-    <t>David_S / Jack</t>
-  </si>
-  <si>
-    <t>Benael / Ricardo</t>
-  </si>
-  <si>
-    <t>Andres / Matt</t>
-  </si>
-  <si>
-    <t>Andres / Yumeng</t>
-  </si>
-  <si>
-    <t>Benael / Rowan</t>
-  </si>
-  <si>
-    <t>Andres / Zeeshan</t>
-  </si>
-  <si>
-    <t>Jack / Ricardo</t>
+    <t>Jack / Yumeng</t>
+  </si>
+  <si>
+    <t>Cedric / Zeeshan</t>
+  </si>
+  <si>
+    <t>Neil / Zeeshan</t>
+  </si>
+  <si>
+    <t>Rowan / Vasisht</t>
+  </si>
+  <si>
+    <t>Ricardo / Vasisht</t>
+  </si>
+  <si>
+    <t>Benael / Zeeshan</t>
+  </si>
+  <si>
+    <t>Rowan / Yumeng</t>
+  </si>
+  <si>
+    <t>David_S / Zeeshan</t>
   </si>
   <si>
     <t>Neil / Yumeng</t>
   </si>
   <si>
-    <t>Matt / Victor</t>
-  </si>
-  <si>
-    <t>Neil / Ricardo</t>
-  </si>
-  <si>
-    <t>Rowan / Zeeshan</t>
-  </si>
-  <si>
-    <t>Jack / Rowan</t>
-  </si>
-  <si>
-    <t>Ricardo / Victor</t>
-  </si>
-  <si>
-    <t>Neil / Victor</t>
-  </si>
-  <si>
-    <t>Matt / Neil</t>
-  </si>
-  <si>
-    <t>Arun / Rowan</t>
+    <t>Ben / Ricardo</t>
+  </si>
+  <si>
+    <t>Ricardo / Rowan</t>
   </si>
   <si>
     <t>Matt / Yumeng</t>
   </si>
   <si>
-    <t>Ricardo / Yumeng</t>
-  </si>
-  <si>
-    <t>Jack / Victor</t>
-  </si>
-  <si>
-    <t>Ricardo / Rowan</t>
-  </si>
-  <si>
-    <t>David_S / Yumeng</t>
-  </si>
-  <si>
-    <t>Jack / Matt</t>
-  </si>
-  <si>
-    <t>Arun / Ricardo</t>
-  </si>
-  <si>
-    <t>Matt / Zeeshan</t>
+    <t>Arun / Ben</t>
+  </si>
+  <si>
+    <t>David_S / Ricardo</t>
+  </si>
+  <si>
+    <t>Matt / Rowan</t>
   </si>
   <si>
     <t>CRAPPR Predicted Best Matchups</t>
@@ -265,53 +274,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D28"/>
+  <dimension ref="B1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="21.453125" style="11" customWidth="true"/>
-    <col min="4" max="4" width="13.453125" style="12" customWidth="true"/>
+    <col min="2" max="3" width="21.7109375" style="11" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" style="12" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" s="13" customFormat="true" ht="20" customHeight="true" x14ac:dyDescent="0.35">
+    <row r="1" s="13" customFormat="true" ht="20" customHeight="true" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" s="14" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" s="14" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" s="15" customFormat="true" ht="27" customHeight="true" x14ac:dyDescent="0.35">
+    <row r="3" s="15" customFormat="true" ht="27" customHeight="true" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" s="16" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.35"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" s="16" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.25"/>
     <row r="5">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D5" s="8">
-        <v>99.92484283447266</v>
+        <v>99.87062072753906</v>
       </c>
     </row>
     <row r="6">
@@ -319,197 +328,197 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8">
-        <v>99.87004852294922</v>
+        <v>99.83395385742188</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8">
-        <v>99.79499053955078</v>
+        <v>99.82241058349609</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="8">
-        <v>99.78539276123047</v>
+        <v>99.71103668212891</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D9" s="8">
-        <v>99.75330352783203</v>
+        <v>99.70591735839844</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D10" s="8">
-        <v>99.74071502685547</v>
+        <v>99.67900085449219</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D11" s="8">
-        <v>99.60501861572266</v>
+        <v>99.67696380615234</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D12" s="8">
-        <v>99.58598327636719</v>
+        <v>99.63908386230469</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="8">
-        <v>99.54397583007813</v>
+        <v>99.54909515380859</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="8">
-        <v>99.45082855224609</v>
+        <v>99.46286773681641</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="8">
-        <v>99.38018798828125</v>
+        <v>99.39426422119141</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="8">
-        <v>99.36785888671875</v>
+        <v>99.35425567626953</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="8">
-        <v>99.32320404052734</v>
+        <v>99.31137847900391</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="8">
-        <v>99.30885314941406</v>
+        <v>99.27555084228516</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="8">
-        <v>99.27179718017578</v>
+        <v>99.22452545166016</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D20" s="8">
-        <v>99.13636779785156</v>
+        <v>99.18723297119141</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D21" s="8">
-        <v>99.02726745605469</v>
+        <v>99.14933776855469</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="7" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="8">
-        <v>98.97199249267578</v>
+        <v>99.13544464111328</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="8">
-        <v>98.9666748046875</v>
+        <v>99.13111877441406</v>
       </c>
     </row>
     <row r="24">
@@ -520,7 +529,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="8">
-        <v>98.80155181884766</v>
+        <v>99.11988830566406</v>
       </c>
     </row>
     <row r="25">
@@ -531,30 +540,63 @@
         <v>34</v>
       </c>
       <c r="D25" s="8">
-        <v>98.75177001953125</v>
-      </c>
-    </row>
-    <row r="26" s="17" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.35">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" s="17" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.35"/>
-    <row r="28" s="18" customFormat="true" ht="39" customHeight="true" x14ac:dyDescent="0.35">
-      <c r="B28" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>39</v>
+        <v>99.11087799072266</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="8">
+        <v>99.04764556884766</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="8">
+        <v>98.95840454101563</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="8">
+        <v>98.92510986328125</v>
+      </c>
+    </row>
+    <row r="29" s="17" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" s="17" customFormat="true" ht="5" customHeight="true" x14ac:dyDescent="0.25"/>
+    <row r="31" s="18" customFormat="true" ht="39" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B31:D31"/>
   </mergeCells>
 </worksheet>
 </file>
</xml_diff>